<commit_message>
Se anexa archivo INVENTARIO.py para, otra forma de desarrollarel problema
</commit_message>
<xml_diff>
--- a/Inventario_ferretería.xlsx
+++ b/Inventario_ferretería.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Téc. Profesional\SEM1\GIt\clase4tecfp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E643E0-A841-4E02-A4BD-2C0B3234F292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9886D93-8673-4E4D-92CC-37D05E341223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Me ayudas creando un Excel con " sheetId="1" r:id="rId1"/>
@@ -104,9 +104,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,11 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -370,7 +368,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -379,8 +377,8 @@
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -396,10 +394,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -419,7 +417,7 @@
       <c r="E2" s="3">
         <v>45225</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>45598</v>
       </c>
     </row>
@@ -439,7 +437,7 @@
       <c r="E3" s="3">
         <v>45225</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>45601</v>
       </c>
     </row>
@@ -459,7 +457,7 @@
       <c r="E4" s="3">
         <v>45225</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>45604</v>
       </c>
     </row>
@@ -479,7 +477,7 @@
       <c r="E5" s="3">
         <v>45225</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>45608</v>
       </c>
     </row>
@@ -499,7 +497,7 @@
       <c r="E6" s="3">
         <v>45225</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>45611</v>
       </c>
     </row>
@@ -519,7 +517,7 @@
       <c r="E7" s="3">
         <v>45225</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>45614</v>
       </c>
     </row>
@@ -539,7 +537,7 @@
       <c r="E8" s="3">
         <v>45225</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>45617</v>
       </c>
     </row>
@@ -559,7 +557,7 @@
       <c r="E9" s="3">
         <v>45225</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>45620</v>
       </c>
     </row>
@@ -579,7 +577,7 @@
       <c r="E10" s="3">
         <v>45225</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>45623</v>
       </c>
     </row>
@@ -599,7 +597,7 @@
       <c r="E11" s="3">
         <v>45225</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>45626</v>
       </c>
     </row>
@@ -619,7 +617,7 @@
       <c r="E12" s="3">
         <v>45225</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>45629</v>
       </c>
     </row>
@@ -639,7 +637,7 @@
       <c r="E13" s="3">
         <v>45225</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>45632</v>
       </c>
     </row>
@@ -659,7 +657,7 @@
       <c r="E14" s="3">
         <v>45225</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>45635</v>
       </c>
     </row>
@@ -679,7 +677,7 @@
       <c r="E15" s="3">
         <v>45225</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>45638</v>
       </c>
     </row>
@@ -699,7 +697,7 @@
       <c r="E16" s="3">
         <v>45225</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>45641</v>
       </c>
     </row>
@@ -719,7 +717,7 @@
       <c r="E17" s="3">
         <v>45225</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>45644</v>
       </c>
     </row>
@@ -739,7 +737,7 @@
       <c r="E18" s="3">
         <v>45225</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>45647</v>
       </c>
     </row>
@@ -759,7 +757,7 @@
       <c r="E19" s="3">
         <v>45225</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>45650</v>
       </c>
     </row>
@@ -779,7 +777,7 @@
       <c r="E20" s="3">
         <v>45225</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>45653</v>
       </c>
     </row>
@@ -799,7 +797,7 @@
       <c r="E21" s="3">
         <v>45225</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>45656</v>
       </c>
     </row>

</xml_diff>